<commit_message>
Modified excels from buys, discs, tickets and givesOpinion
</commit_message>
<xml_diff>
--- a/Archivos Excel/buysDiscs.xlsx
+++ b/Archivos Excel/buysDiscs.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E04AE0-0C96-4D53-BB54-DD8A64BE49BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62ECEE9C-5EA6-445D-96E2-94AA113B0221}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23940" windowHeight="9465" xr2:uid="{D1AA7CAB-F191-4E72-9401-29BC742C93A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$20:$B$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -74,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA30E138-CCEA-416E-929B-DCE5AC404A36}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,14 +504,603 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1238471</v>
+      </c>
+      <c r="B21">
+        <v>1203</v>
+      </c>
+      <c r="F21" t="str">
+        <f>CONCATENATE($I$1,$C$20,A21,$K$1,B21,$J$1)</f>
+        <v>insert into buysDisc values(01238471,1203);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1238471</v>
+      </c>
+      <c r="B22">
+        <v>8892</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" ref="F22:F67" si="0">CONCATENATE($I$1,$C$20,A22,$K$1,B22,$J$1)</f>
+        <v>insert into buysDisc values(01238471,8892);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1238471</v>
+      </c>
+      <c r="B23">
+        <v>3627</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(01238471,3627);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1238471</v>
+      </c>
+      <c r="B24">
+        <v>7329</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(01238471,7329);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2321423</v>
+      </c>
+      <c r="B25">
+        <v>2056</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02321423,2056);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2321423</v>
+      </c>
+      <c r="B26">
+        <v>2984</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02321423,2984);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2321423</v>
+      </c>
+      <c r="B27">
+        <v>1784</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02321423,1784);</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2321423</v>
+      </c>
+      <c r="B28">
+        <v>3282</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02321423,3282);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2321423</v>
+      </c>
+      <c r="B29">
+        <v>7482</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02321423,7482);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2374827</v>
+      </c>
+      <c r="B30">
+        <v>7329</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02374827,7329);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2374827</v>
+      </c>
+      <c r="B31">
+        <v>5738</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02374827,5738);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2374827</v>
+      </c>
+      <c r="B32">
+        <v>7231</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02374827,7231);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2374827</v>
+      </c>
+      <c r="B33">
+        <v>7482</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(02374827,7482);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3283295</v>
+      </c>
+      <c r="B34">
+        <v>6234</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(03283295,6234);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3283295</v>
+      </c>
+      <c r="B35">
+        <v>6321</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(03283295,6321);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3421987</v>
+      </c>
+      <c r="B36">
+        <v>7482</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(03421987,7482);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3421987</v>
+      </c>
+      <c r="B37">
+        <v>7231</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(03421987,7231);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3421987</v>
+      </c>
+      <c r="B38">
+        <v>6321</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(03421987,6321);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4309871</v>
+      </c>
+      <c r="B39">
+        <v>7482</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04309871,7482);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4309871</v>
+      </c>
+      <c r="B40">
+        <v>5738</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04309871,5738);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4309871</v>
+      </c>
+      <c r="B41">
+        <v>6234</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04309871,6234);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>4528483</v>
+      </c>
+      <c r="B42">
+        <v>2984</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04528483,2984);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>4528483</v>
+      </c>
+      <c r="B43">
+        <v>1203</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04528483,1203);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>4528483</v>
+      </c>
+      <c r="B44">
+        <v>8892</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04528483,8892);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>4528483</v>
+      </c>
+      <c r="B45">
+        <v>3627</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="F45" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04528483,3627);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>4737492</v>
+      </c>
+      <c r="B46">
+        <v>3282</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="F46" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04737492,3282);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>4737492</v>
+      </c>
+      <c r="B47">
+        <v>6234</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04737492,6234);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>4782107</v>
+      </c>
+      <c r="B48">
+        <v>7329</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04782107,7329);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4782107</v>
+      </c>
+      <c r="B49">
+        <v>7231</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04782107,7231);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>4782107</v>
+      </c>
+      <c r="B50">
+        <v>3492</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04782107,3492);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>4917493</v>
+      </c>
+      <c r="B51">
+        <v>2984</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="F51" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04917493,2984);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>4917493</v>
+      </c>
+      <c r="B52">
+        <v>1203</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="F52" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04917493,1203);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>4917493</v>
+      </c>
+      <c r="B53">
+        <v>5738</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="F53" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04917493,5738);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>4917493</v>
+      </c>
+      <c r="B54">
+        <v>7231</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="F54" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(04917493,7231);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5838743</v>
+      </c>
+      <c r="B55">
+        <v>3627</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="F55" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(05838743,3627);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>5838743</v>
+      </c>
+      <c r="B56">
+        <v>7329</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="F56" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(05838743,7329);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5838743</v>
+      </c>
+      <c r="B57">
+        <v>6234</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="F57" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(05838743,6234);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>5838743</v>
+      </c>
+      <c r="B58">
+        <v>7231</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="F58" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(05838743,7231);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>9043278</v>
+      </c>
+      <c r="B59">
+        <v>8892</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="F59" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09043278,8892);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>9043278</v>
+      </c>
+      <c r="B60">
+        <v>7482</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09043278,7482);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>9043278</v>
+      </c>
+      <c r="B61">
+        <v>5738</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09043278,5738);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>9043278</v>
+      </c>
+      <c r="B62">
+        <v>7329</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09043278,7329);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>9043278</v>
+      </c>
+      <c r="B63">
+        <v>6321</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09043278,6321);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>9043278</v>
+      </c>
+      <c r="B64">
+        <v>7482</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09043278,7482);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>9373493</v>
+      </c>
+      <c r="B65">
+        <v>8892</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09373493,8892);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>9373493</v>
+      </c>
+      <c r="B66">
+        <v>3282</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09373493,3282);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>9373493</v>
+      </c>
+      <c r="B67">
+        <v>3229</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into buysDisc values(09373493,3229);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>